<commit_message>
Update points 79172233 -> 30.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>birthday</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_points</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -454,6 +459,9 @@
           <t>2015-08-26</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -464,6 +472,9 @@
           <t>2025-09-08</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -474,17 +485,21 @@
           <t>1960-08-16</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>79172233</t>
-        </is>
+      <c r="A5" t="n">
+        <v>79172233</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>2025-08-10</t>
         </is>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update points 79174445 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -503,10 +503,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>79174445</t>
-        </is>
+      <c r="A6" t="n">
+        <v>79174445</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update points 71277628 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -527,10 +527,8 @@
       <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>71277628</t>
-        </is>
+      <c r="A8" t="n">
+        <v>71277628</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update points 71277620 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -540,10 +540,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>71277620</t>
-        </is>
+      <c r="A9" t="n">
+        <v>71277620</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update points 71076783 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,6 +552,17 @@
         <v>1164</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>71076783</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 71076781 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,17 @@
         <v>100</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>71076781</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 09876543 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +570,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 09876543 -> 120.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -718,14 +718,23 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A27" t="n">
+        <v>9876543</v>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>09876543</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update points 76442781 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -1049,10 +1049,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>09876543</t>
-        </is>
+      <c r="A62" t="n">
+        <v>9876543</v>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="n">

</xml_diff>

<commit_message>
Update points 51616172 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1057,6 +1057,17 @@
         <v>120</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>51616172</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 51616176 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1066,6 +1066,17 @@
         <v>120</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>51616176</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 51616170 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1075,6 +1075,17 @@
         <v>125</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>51616170</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 51616162 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1084,6 +1084,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>51616162</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 51616191 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1093,6 +1093,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>51616191</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 71717171 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1106,6 +1106,17 @@
         <v>140</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>71717171</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 71717172 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1119,6 +1119,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>71717172</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 71717170 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1132,6 +1132,17 @@
         <v>125</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>71717170</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 71717179 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,6 +1145,17 @@
         <v>264</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>71717179</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 71717173 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1154,6 +1154,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>71717173</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 76442711 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1167,6 +1167,17 @@
         <v>751</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>76442711</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 76442711 -> 408.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -451,10 +451,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>76442711</t>
-        </is>
+      <c r="A2" t="n">
+        <v>76442711</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -462,7 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reset customers.xlsx (clear all data)
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,19 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>76442711</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2000-08-24</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>816</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174441 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>79174441</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174442 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>79174442</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174421 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>79174421</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174401 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>79174401</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174404 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>79174404</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174409 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,6 +538,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>79174409</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174408 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,6 +547,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>79174408</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174414 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>79174414</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174418 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>79174418</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174419 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,6 +578,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>79174419</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174463 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>79174463</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174466 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -600,6 +600,17 @@
         <v>40</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>79174466</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174460 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +609,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>79174460</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update points 79174449 -> 0.00
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,6 +626,17 @@
         <v>50</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>79174449</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>